<commit_message>
Preparing for cooperation on new parser
</commit_message>
<xml_diff>
--- a/data/Mahlon/C_1760_070_FINAL.xlsx
+++ b/data/Mahlon/C_1760_070_FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1king\Senior Design Repos\shoppingstories-parser\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1king\Senior Design Repos\shoppingstories-parser\data\Mahlon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8176E854-277A-4D13-A942-CF70DA1A5FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E89FBE-F898-4CF8-8CB6-803D151E09DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8415" yWindow="4350" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="186">
   <si>
     <t>Sterling</t>
   </si>
@@ -641,9 +641,6 @@
   </si>
   <si>
     <t>Reviewer 2: N. Resch/0.25</t>
-  </si>
-  <si>
-    <t>To ¼ red green Rum 1/6</t>
   </si>
 </sst>
 </file>
@@ -1410,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
@@ -1419,20 +1416,27 @@
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.875" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.75" style="1" customWidth="1"/>
-    <col min="11" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="16" width="9.125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="5.125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="0.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="0.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="1" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1" style="1" customWidth="1"/>
+    <col min="13" max="13" width="1.25" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="1.25" style="1" customWidth="1"/>
+    <col min="16" max="16" width="1" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3" style="1" customWidth="1"/>
+    <col min="18" max="18" width="0.875" style="1" customWidth="1"/>
     <col min="19" max="19" width="5.625" style="1" customWidth="1"/>
-    <col min="20" max="21" width="6.125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="1.25" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.125" style="1" customWidth="1"/>
     <col min="22" max="22" width="5.625" style="1" customWidth="1"/>
     <col min="23" max="23" width="32.25" style="2" customWidth="1"/>
-    <col min="24" max="24" width="9.375" style="1" customWidth="1"/>
-    <col min="25" max="26" width="7" style="1" customWidth="1"/>
+    <col min="24" max="24" width="0.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5" style="1" customWidth="1"/>
+    <col min="26" max="26" width="7" style="1" customWidth="1"/>
     <col min="27" max="27" width="3.875" style="1" customWidth="1"/>
     <col min="28" max="28" width="5.625" style="1" customWidth="1"/>
     <col min="29" max="29" width="5.75" style="1" customWidth="1"/>
@@ -2075,7 +2079,7 @@
       </c>
       <c r="AO6" s="20"/>
     </row>
-    <row r="7" spans="1:41" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" s="21" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
       <c r="B7" s="27"/>
       <c r="C7" s="14" t="s">
@@ -2525,7 +2529,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:41" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" s="21" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="22"/>
       <c r="C11" s="14" t="s">
@@ -4654,7 +4658,7 @@
       <c r="AN29" s="20"/>
       <c r="AO29" s="20"/>
     </row>
-    <row r="30" spans="1:41" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" s="21" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="22"/>
       <c r="C30" s="14" t="s">
@@ -4716,7 +4720,7 @@
         <v>145</v>
       </c>
       <c r="W30" s="15" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>21</v>
@@ -6335,7 +6339,7 @@
       <c r="AN44" s="20"/>
       <c r="AO44" s="20"/>
     </row>
-    <row r="45" spans="1:41" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" s="21" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="22"/>
       <c r="C45" s="14" t="s">

</xml_diff>